<commit_message>
Added type hints, moved code to create dictionary with multiple dataframes to a function
</commit_message>
<xml_diff>
--- a/sample data/Sample EU Supreme Products for the Week of September 15 2022 (Week 4 of FW22) - Sheets.xlsx
+++ b/sample data/Sample EU Supreme Products for the Week of September 15 2022 (Week 4 of FW22) - Sheets.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huymai/Desktop/supreme-products-scraper/sample data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F483ABE-0482-9341-9112-A142FAEF090A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bags" sheetId="1" r:id="rId1"/>
@@ -13,13 +19,13 @@
     <sheet name="Pants" sheetId="4" r:id="rId4"/>
     <sheet name="Shorts" sheetId="5" r:id="rId5"/>
     <sheet name="Tops_Sweaters" sheetId="6" r:id="rId6"/>
-    <sheet name="T_Shirts" sheetId="7" r:id="rId7"/>
+    <sheet name="T-Shirts" sheetId="7" r:id="rId7"/>
     <sheet name="Jackets" sheetId="8" r:id="rId8"/>
     <sheet name="Sweatshirts" sheetId="9" r:id="rId9"/>
     <sheet name="Hats" sheetId="10" r:id="rId10"/>
     <sheet name="Accessories" sheetId="11" r:id="rId11"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -1373,8 +1379,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1437,6 +1443,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1483,7 +1497,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1515,9 +1529,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1549,6 +1581,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1724,14 +1774,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1778,7 +1828,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1825,7 +1875,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1872,7 +1922,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1919,7 +1969,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1966,7 +2016,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -2013,7 +2063,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -2066,14 +2116,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2120,7 +2170,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>366</v>
       </c>
@@ -2167,7 +2217,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>367</v>
       </c>
@@ -2214,7 +2264,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>368</v>
       </c>
@@ -2261,7 +2311,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>369</v>
       </c>
@@ -2308,7 +2358,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>370</v>
       </c>
@@ -2355,7 +2405,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>371</v>
       </c>
@@ -2402,7 +2452,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>372</v>
       </c>
@@ -2455,14 +2505,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2509,7 +2559,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>409</v>
       </c>
@@ -2556,7 +2606,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>410</v>
       </c>
@@ -2603,7 +2653,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>411</v>
       </c>
@@ -2650,7 +2700,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>412</v>
       </c>
@@ -2697,7 +2747,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>413</v>
       </c>
@@ -2744,7 +2794,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>414</v>
       </c>
@@ -2791,7 +2841,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>415</v>
       </c>
@@ -2844,14 +2894,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2898,7 +2948,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -2945,7 +2995,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -2992,7 +3042,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>55</v>
       </c>
@@ -3039,7 +3089,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>56</v>
       </c>
@@ -3092,14 +3142,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3146,7 +3196,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>82</v>
       </c>
@@ -3193,7 +3243,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>83</v>
       </c>
@@ -3240,7 +3290,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -3284,7 +3334,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>85</v>
       </c>
@@ -3337,14 +3387,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3391,7 +3441,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -3438,7 +3488,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>108</v>
       </c>
@@ -3485,7 +3535,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>109</v>
       </c>
@@ -3532,7 +3582,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -3579,7 +3629,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>111</v>
       </c>
@@ -3626,7 +3676,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>112</v>
       </c>
@@ -3673,7 +3723,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>113</v>
       </c>
@@ -3720,7 +3770,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>114</v>
       </c>
@@ -3767,7 +3817,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>115</v>
       </c>
@@ -3814,7 +3864,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>116</v>
       </c>
@@ -3861,7 +3911,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>117</v>
       </c>
@@ -3914,14 +3964,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3968,7 +4018,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>176</v>
       </c>
@@ -4015,7 +4065,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>177</v>
       </c>
@@ -4068,14 +4118,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4122,7 +4172,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>189</v>
       </c>
@@ -4169,7 +4219,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>190</v>
       </c>
@@ -4216,7 +4266,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>191</v>
       </c>
@@ -4263,7 +4313,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>192</v>
       </c>
@@ -4310,7 +4360,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>193</v>
       </c>
@@ -4357,7 +4407,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>194</v>
       </c>
@@ -4404,7 +4454,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>195</v>
       </c>
@@ -4451,7 +4501,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>196</v>
       </c>
@@ -4498,7 +4548,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>197</v>
       </c>
@@ -4545,7 +4595,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>198</v>
       </c>
@@ -4592,7 +4642,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>199</v>
       </c>
@@ -4645,14 +4695,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4699,7 +4749,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>256</v>
       </c>
@@ -4746,7 +4796,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>257</v>
       </c>
@@ -4793,7 +4843,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>258</v>
       </c>
@@ -4840,7 +4890,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>259</v>
       </c>
@@ -4887,7 +4937,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>260</v>
       </c>
@@ -4940,14 +4990,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4994,7 +5044,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>286</v>
       </c>
@@ -5041,7 +5091,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>287</v>
       </c>
@@ -5088,7 +5138,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>288</v>
       </c>
@@ -5135,7 +5185,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>289</v>
       </c>
@@ -5182,7 +5232,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>290</v>
       </c>
@@ -5229,7 +5279,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>291</v>
       </c>
@@ -5282,14 +5332,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5336,7 +5386,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>323</v>
       </c>
@@ -5383,7 +5433,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>324</v>
       </c>
@@ -5430,7 +5480,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>325</v>
       </c>
@@ -5477,7 +5527,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>326</v>
       </c>
@@ -5524,7 +5574,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>327</v>
       </c>
@@ -5571,7 +5621,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>328</v>
       </c>
@@ -5618,7 +5668,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>329</v>
       </c>

</xml_diff>